<commit_message>
fixed an error in this
</commit_message>
<xml_diff>
--- a/avverages page added.xlsx
+++ b/avverages page added.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="District Data By Days" sheetId="1" r:id="rId1"/>
@@ -5413,8 +5413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK36"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AK35" sqref="AK2:AK35"/>
+    <sheetView topLeftCell="AA9" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2:AK35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5639,8 +5639,8 @@
         <v>0</v>
       </c>
       <c r="AK2" s="2">
-        <f t="shared" ref="AK2:AK35" si="0">SUM(B2:AJ2)</f>
-        <v>1.0235700000000001</v>
+        <f t="shared" ref="AK2:AK35" si="0">AVERAGE(B2:AJ2)</f>
+        <v>2.9244857142857145E-2</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="AK3" s="2">
         <f t="shared" si="0"/>
-        <v>0.11500000000000005</v>
+        <v>3.2857142857142872E-3</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="AK4" s="2">
         <f t="shared" si="0"/>
-        <v>1.0579599999999998</v>
+        <v>3.0227428571428565E-2</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="AK5" s="2">
         <f t="shared" si="0"/>
-        <v>1.5594899999999998</v>
+        <v>4.4556857142857141E-2</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
@@ -6096,7 +6096,7 @@
       </c>
       <c r="AK6" s="2">
         <f t="shared" si="0"/>
-        <v>0.15413000000000002</v>
+        <v>4.403714285714286E-3</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -6210,7 +6210,7 @@
       </c>
       <c r="AK7" s="2">
         <f t="shared" si="0"/>
-        <v>0.78699999999999992</v>
+        <v>2.2485714285714282E-2</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -6324,7 +6324,7 @@
       </c>
       <c r="AK8" s="2">
         <f t="shared" si="0"/>
-        <v>0.98881999999999981</v>
+        <v>2.8251999999999996E-2</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="AK9" s="2">
         <f t="shared" si="0"/>
-        <v>0.28500000000000003</v>
+        <v>8.1428571428571444E-3</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -6552,7 +6552,7 @@
       </c>
       <c r="AK10" s="2">
         <f t="shared" si="0"/>
-        <v>2.25373</v>
+        <v>6.4392285714285721E-2</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="AK11" s="2">
         <f t="shared" si="0"/>
-        <v>3.0670000000000002</v>
+        <v>8.7628571428571431E-2</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="AK12" s="2">
         <f t="shared" si="0"/>
-        <v>0.89127000000000045</v>
+        <v>2.5464857142857157E-2</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
@@ -6894,7 +6894,7 @@
       </c>
       <c r="AK13" s="2">
         <f t="shared" si="0"/>
-        <v>4.859799999999999</v>
+        <v>0.13885142857142854</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -7008,7 +7008,7 @@
       </c>
       <c r="AK14" s="2">
         <f t="shared" si="0"/>
-        <v>0.67662999999999995</v>
+        <v>1.9332285714285712E-2</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -7122,7 +7122,7 @@
       </c>
       <c r="AK15" s="2">
         <f t="shared" si="0"/>
-        <v>0.95940999999999999</v>
+        <v>2.7411714285714286E-2</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -7236,7 +7236,7 @@
       </c>
       <c r="AK16" s="2">
         <f t="shared" si="0"/>
-        <v>0.5950000000000002</v>
+        <v>1.7000000000000005E-2</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
@@ -7350,7 +7350,7 @@
       </c>
       <c r="AK17" s="2">
         <f t="shared" si="0"/>
-        <v>0.18539000000000005</v>
+        <v>5.2968571428571448E-3</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -7464,7 +7464,7 @@
       </c>
       <c r="AK18" s="2">
         <f t="shared" si="0"/>
-        <v>3.9949999999999999E-2</v>
+        <v>1.1414285714285714E-3</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
@@ -7578,7 +7578,7 @@
       </c>
       <c r="AK19" s="2">
         <f t="shared" si="0"/>
-        <v>1.0112300000000001</v>
+        <v>2.8892285714285718E-2</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
@@ -7692,7 +7692,7 @@
       </c>
       <c r="AK20" s="2">
         <f t="shared" si="0"/>
-        <v>7.8369700000000009</v>
+        <v>0.2239134285714286</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
@@ -7806,7 +7806,7 @@
       </c>
       <c r="AK21" s="2">
         <f t="shared" si="0"/>
-        <v>0.10795000000000002</v>
+        <v>3.0842857142857148E-3</v>
       </c>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="AK22" s="2">
         <f t="shared" si="0"/>
-        <v>1.10588</v>
+        <v>3.1596571428571425E-2</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
@@ -8034,7 +8034,7 @@
       </c>
       <c r="AK23" s="2">
         <f t="shared" si="0"/>
-        <v>0.11645000000000001</v>
+        <v>3.3271428571428575E-3</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -8148,7 +8148,7 @@
       </c>
       <c r="AK24" s="2">
         <f t="shared" si="0"/>
-        <v>8.900000000000001E-2</v>
+        <v>2.5428571428571431E-3</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
@@ -8262,7 +8262,7 @@
       </c>
       <c r="AK25" s="2">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>2.8571428571428571E-3</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
@@ -8376,7 +8376,7 @@
       </c>
       <c r="AK26" s="2">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>1.1428571428571429E-3</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
@@ -8604,7 +8604,7 @@
       </c>
       <c r="AK28" s="2">
         <f t="shared" si="0"/>
-        <v>2.494E-2</v>
+        <v>7.1257142857142862E-4</v>
       </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
@@ -8718,7 +8718,7 @@
       </c>
       <c r="AK29" s="2">
         <f t="shared" si="0"/>
-        <v>7.3409999999999989E-2</v>
+        <v>2.0974285714285713E-3</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
@@ -9174,7 +9174,7 @@
       </c>
       <c r="AK33" s="2">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>5.7142857142857147E-4</v>
       </c>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
@@ -9288,7 +9288,7 @@
       </c>
       <c r="AK34" s="2">
         <f t="shared" si="0"/>
-        <v>1.1990000000000001E-2</v>
+        <v>3.4257142857142857E-4</v>
       </c>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
@@ -31390,7 +31390,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31429,7 +31429,7 @@
         <v>1.7003142857142862E-2</v>
       </c>
       <c r="C2">
-        <v>1.0235700000000001</v>
+        <v>2.9244857142857145E-2</v>
       </c>
       <c r="D2">
         <v>1.6164571428571431E-2</v>
@@ -31455,7 +31455,7 @@
         <v>2.1428571428571434E-3</v>
       </c>
       <c r="C3">
-        <v>0.11500000000000005</v>
+        <v>3.2857142857142872E-3</v>
       </c>
       <c r="D3">
         <v>3.4285714285714297E-3</v>
@@ -31481,7 +31481,7 @@
         <v>4.9346857142857144E-2</v>
       </c>
       <c r="C4">
-        <v>1.0579599999999998</v>
+        <v>3.0227428571428565E-2</v>
       </c>
       <c r="D4">
         <v>5.2784285714285714E-2</v>
@@ -31507,7 +31507,7 @@
         <v>3.0250857142857145E-2</v>
       </c>
       <c r="C5">
-        <v>1.5594899999999998</v>
+        <v>4.4556857142857141E-2</v>
       </c>
       <c r="D5">
         <v>4.2203428571428565E-2</v>
@@ -31533,7 +31533,7 @@
         <v>4.4514285714285715E-3</v>
       </c>
       <c r="C6">
-        <v>0.15413000000000002</v>
+        <v>4.403714285714286E-3</v>
       </c>
       <c r="D6">
         <v>3.5391428571428575E-3</v>
@@ -31559,7 +31559,7 @@
         <v>1.8828571428571427E-2</v>
       </c>
       <c r="C7">
-        <v>0.78699999999999992</v>
+        <v>2.2485714285714282E-2</v>
       </c>
       <c r="D7">
         <v>2.1885714285714283E-2</v>
@@ -31585,7 +31585,7 @@
         <v>1.9486285714285716E-2</v>
       </c>
       <c r="C8">
-        <v>0.98881999999999981</v>
+        <v>2.8251999999999996E-2</v>
       </c>
       <c r="D8">
         <v>1.9661142857142856E-2</v>
@@ -31611,7 +31611,7 @@
         <v>1.1314285714285712E-2</v>
       </c>
       <c r="C9">
-        <v>0.28500000000000003</v>
+        <v>8.1428571428571444E-3</v>
       </c>
       <c r="D9">
         <v>4.8599999999999997E-2</v>
@@ -31637,7 +31637,7 @@
         <v>4.725628571428573E-2</v>
       </c>
       <c r="C10">
-        <v>2.25373</v>
+        <v>6.4392285714285721E-2</v>
       </c>
       <c r="D10">
         <v>5.2703714285714277E-2</v>
@@ -31663,7 +31663,7 @@
         <v>5.8628571428571405E-2</v>
       </c>
       <c r="C11">
-        <v>3.0670000000000002</v>
+        <v>8.7628571428571431E-2</v>
       </c>
       <c r="D11">
         <v>6.6871428571428568E-2</v>
@@ -31689,7 +31689,7 @@
         <v>2.0755714285714294E-2</v>
       </c>
       <c r="C12">
-        <v>0.89127000000000045</v>
+        <v>2.5464857142857157E-2</v>
       </c>
       <c r="D12">
         <v>1.592514285714286E-2</v>
@@ -31715,7 +31715,7 @@
         <v>9.3269999999999992E-2</v>
       </c>
       <c r="C13">
-        <v>4.859799999999999</v>
+        <v>0.13885142857142854</v>
       </c>
       <c r="D13">
         <v>0.11710514285714285</v>
@@ -31741,7 +31741,7 @@
         <v>4.9156571428571438E-2</v>
       </c>
       <c r="C14">
-        <v>0.67662999999999995</v>
+        <v>1.9332285714285712E-2</v>
       </c>
       <c r="D14">
         <v>1.7652571428571431E-2</v>
@@ -31767,7 +31767,7 @@
         <v>5.8533714285714272E-2</v>
       </c>
       <c r="C15">
-        <v>0.95940999999999999</v>
+        <v>2.7411714285714286E-2</v>
       </c>
       <c r="D15">
         <v>2.2870571428571424E-2</v>
@@ -31793,7 +31793,7 @@
         <v>1.6400000000000005E-2</v>
       </c>
       <c r="C16">
-        <v>0.5950000000000002</v>
+        <v>1.7000000000000005E-2</v>
       </c>
       <c r="D16">
         <v>1.542857142857143E-2</v>
@@ -31819,7 +31819,7 @@
         <v>3.5119999999999999E-3</v>
       </c>
       <c r="C17">
-        <v>0.18539000000000005</v>
+        <v>5.2968571428571448E-3</v>
       </c>
       <c r="D17">
         <v>3.4262857142857146E-3</v>
@@ -31845,7 +31845,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>3.9949999999999999E-2</v>
+        <v>1.1414285714285714E-3</v>
       </c>
       <c r="D18">
         <v>3.9971428571428574E-4</v>
@@ -31871,7 +31871,7 @@
         <v>1.6150285714285718E-2</v>
       </c>
       <c r="C19">
-        <v>1.0112300000000001</v>
+        <v>2.8892285714285718E-2</v>
       </c>
       <c r="D19">
         <v>1.9283142857142856E-2</v>
@@ -31897,7 +31897,7 @@
         <v>0.20812000000000003</v>
       </c>
       <c r="C20">
-        <v>7.8369700000000009</v>
+        <v>0.2239134285714286</v>
       </c>
       <c r="D20">
         <v>0.2637828571428571</v>
@@ -31923,7 +31923,7 @@
         <v>4.8254285714285708E-3</v>
       </c>
       <c r="C21">
-        <v>0.10795000000000002</v>
+        <v>3.0842857142857148E-3</v>
       </c>
       <c r="D21">
         <v>2.2597142857142855E-3</v>
@@ -31949,7 +31949,7 @@
         <v>5.3953142857142866E-2</v>
       </c>
       <c r="C22">
-        <v>1.10588</v>
+        <v>3.1596571428571425E-2</v>
       </c>
       <c r="D22">
         <v>3.3526571428571419E-2</v>
@@ -31975,7 +31975,7 @@
         <v>5.230571428571429E-3</v>
       </c>
       <c r="C23">
-        <v>0.11645000000000001</v>
+        <v>3.3271428571428575E-3</v>
       </c>
       <c r="D23">
         <v>2.5685714285714287E-4</v>
@@ -32001,7 +32001,7 @@
         <v>7.9999999999999993E-4</v>
       </c>
       <c r="C24">
-        <v>8.900000000000001E-2</v>
+        <v>2.5428571428571431E-3</v>
       </c>
       <c r="D24">
         <v>3.9257142857142854E-4</v>
@@ -32027,7 +32027,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0.1</v>
+        <v>2.8571428571428571E-3</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -32053,7 +32053,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.04</v>
+        <v>1.1428571428571429E-3</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -32105,7 +32105,7 @@
         <v>9.4500000000000001E-3</v>
       </c>
       <c r="C28">
-        <v>2.494E-2</v>
+        <v>7.1257142857142862E-4</v>
       </c>
       <c r="D28">
         <v>2.1102857142857143E-3</v>
@@ -32131,7 +32131,7 @@
         <v>1.6071428571428569E-3</v>
       </c>
       <c r="C29">
-        <v>7.3409999999999989E-2</v>
+        <v>2.0974285714285713E-3</v>
       </c>
       <c r="D29">
         <v>8.5368571428571429E-3</v>
@@ -32235,7 +32235,7 @@
         <v>8.571428571428571E-4</v>
       </c>
       <c r="C33">
-        <v>0.02</v>
+        <v>5.7142857142857147E-4</v>
       </c>
       <c r="D33">
         <v>3.7142857142857143E-4</v>
@@ -32261,7 +32261,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>1.1990000000000001E-2</v>
+        <v>3.4257142857142857E-4</v>
       </c>
       <c r="D34">
         <v>0</v>

</xml_diff>